<commit_message>
Actualizacion Cliente 1 y más analisis explora
</commit_message>
<xml_diff>
--- a/Datos Electro Dunas/sector_economico_clientes.xlsx
+++ b/Datos Electro Dunas/sector_economico_clientes.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/n_pacheco10_uniandes_edu_co/Documents/0. AnalíticaGEB/caso_electrodunas/Datos_reto/Datos Reto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{DE6CDB19-91E3-4CA8-A6A1-B2D7C53902CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F4B9D8-A2F1-493E-8CFD-6306C514993B}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{DE6CDB19-91E3-4CA8-A6A1-B2D7C53902CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F4B9D8-A2F1-493E-8CFD-6306C514993B}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11505" xr2:uid="{2C301879-9D78-444A-AEC6-03709C14F396}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -41,125 +30,125 @@
     <t>Cliente:</t>
   </si>
   <si>
+    <t xml:space="preserve">Cliente 1 </t>
+  </si>
+  <si>
+    <t>Cliente 2</t>
+  </si>
+  <si>
+    <t>Cliente 3</t>
+  </si>
+  <si>
+    <t>Cliente 4</t>
+  </si>
+  <si>
+    <t>Cliente 5</t>
+  </si>
+  <si>
+    <t>Cliente 6</t>
+  </si>
+  <si>
+    <t>Cliente 7</t>
+  </si>
+  <si>
+    <t>Cliente 8</t>
+  </si>
+  <si>
+    <t>Cliente 9</t>
+  </si>
+  <si>
+    <t>Cliente 10</t>
+  </si>
+  <si>
+    <t>Cliente 11</t>
+  </si>
+  <si>
+    <t>Cliente 12</t>
+  </si>
+  <si>
+    <t>Cliente 13</t>
+  </si>
+  <si>
+    <t>Cliente 14</t>
+  </si>
+  <si>
+    <t>Cliente 15</t>
+  </si>
+  <si>
+    <t>Cliente 16</t>
+  </si>
+  <si>
+    <t>Cliente 17</t>
+  </si>
+  <si>
+    <t>Cliente 18</t>
+  </si>
+  <si>
+    <t>Cliente 19</t>
+  </si>
+  <si>
+    <t>Cliente 20</t>
+  </si>
+  <si>
+    <t>Cliente 21</t>
+  </si>
+  <si>
+    <t>Cliente 22</t>
+  </si>
+  <si>
+    <t>Cliente 23</t>
+  </si>
+  <si>
+    <t>Cliente 24</t>
+  </si>
+  <si>
+    <t>Cliente 25</t>
+  </si>
+  <si>
+    <t>Cliente 26</t>
+  </si>
+  <si>
+    <t>Cliente 27</t>
+  </si>
+  <si>
+    <t>Cliente 28</t>
+  </si>
+  <si>
+    <t>Cliente 29</t>
+  </si>
+  <si>
+    <t>Cliente 30</t>
+  </si>
+  <si>
     <t>Sector Económico:</t>
   </si>
   <si>
-    <t xml:space="preserve">Cliente 1 </t>
+    <t>Venta al por mayor de metales y minerales metalíferos</t>
   </si>
   <si>
     <t>Elaboración de cacao y chocolate y de productos de confitería</t>
   </si>
   <si>
-    <t>Cliente 2</t>
-  </si>
-  <si>
-    <t>Cliente 3</t>
-  </si>
-  <si>
-    <t>Cliente 4</t>
-  </si>
-  <si>
-    <t>Cliente 5</t>
-  </si>
-  <si>
-    <t>Cliente 6</t>
+    <t>Cultivo de otros frutos y nueces de árboles y arbustos</t>
+  </si>
+  <si>
+    <t>Cultivo de hortalizas y melones, raíces y tubérculos</t>
   </si>
   <si>
     <t>Cultivo de Árboles Frutales y Nueces</t>
   </si>
   <si>
-    <t>Cliente 7</t>
-  </si>
-  <si>
-    <t>Cliente 8</t>
-  </si>
-  <si>
-    <t>Cliente 9</t>
-  </si>
-  <si>
-    <t>Cliente 10</t>
-  </si>
-  <si>
-    <t>Cliente 11</t>
-  </si>
-  <si>
-    <t>Cultivo de otros frutos y nueces de árboles y arbustos</t>
-  </si>
-  <si>
-    <t>Cliente 12</t>
-  </si>
-  <si>
-    <t>Cliente 13</t>
-  </si>
-  <si>
-    <t>Cultivo de hortalizas y melones, raíces y tubérculos</t>
-  </si>
-  <si>
-    <t>Cliente 14</t>
-  </si>
-  <si>
-    <t>Cliente 15</t>
-  </si>
-  <si>
-    <t>Cliente 16</t>
+    <t>Cultivo de Hortalizas</t>
   </si>
   <si>
     <t>Captación, tratamiento y distribución de agua</t>
-  </si>
-  <si>
-    <t>Cliente 17</t>
-  </si>
-  <si>
-    <t>Cliente 18</t>
-  </si>
-  <si>
-    <t>Cliente 19</t>
-  </si>
-  <si>
-    <t>Cliente 20</t>
-  </si>
-  <si>
-    <t>Cliente 21</t>
-  </si>
-  <si>
-    <t>Cultivo de Hortalizas</t>
-  </si>
-  <si>
-    <t>Cliente 22</t>
-  </si>
-  <si>
-    <t>Cliente 23</t>
-  </si>
-  <si>
-    <t>Cliente 24</t>
-  </si>
-  <si>
-    <t>Cliente 25</t>
-  </si>
-  <si>
-    <t>Cliente 26</t>
-  </si>
-  <si>
-    <t>Venta al por mayor de metales y minerales metalíferos</t>
-  </si>
-  <si>
-    <t>Cliente 27</t>
-  </si>
-  <si>
-    <t>Cliente 28</t>
-  </si>
-  <si>
-    <t>Cliente 29</t>
-  </si>
-  <si>
-    <t>Cliente 30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -534,258 +523,258 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -795,23 +784,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c92cab73-d3fa-463d-b5ac-11fb3a3bdd22" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000E1E61A266C41A4AB4AB44994D2CC70D" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5b0c2a764da195df8b1f6cbadad6c104">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c92cab73-d3fa-463d-b5ac-11fb3a3bdd22" xmlns:ns4="e5f8797d-9fae-4fdb-a6e2-340a0c59bf88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="935b2b7abf65da668dcdde7753a5ff04" ns3:_="" ns4:_="">
     <xsd:import namespace="c92cab73-d3fa-463d-b5ac-11fb3a3bdd22"/>
@@ -1058,14 +1030,63 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c92cab73-d3fa-463d-b5ac-11fb3a3bdd22" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54C957E8-572F-4EAF-8EEE-BD6FA4964C19}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1530DB57-D452-43FD-83E5-8657E4020787}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c92cab73-d3fa-463d-b5ac-11fb3a3bdd22"/>
+    <ds:schemaRef ds:uri="e5f8797d-9fae-4fdb-a6e2-340a0c59bf88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F60AE1-65D5-47E3-8428-C27860B18F62}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15F60AE1-65D5-47E3-8428-C27860B18F62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1530DB57-D452-43FD-83E5-8657E4020787}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54C957E8-572F-4EAF-8EEE-BD6FA4964C19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e5f8797d-9fae-4fdb-a6e2-340a0c59bf88"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c92cab73-d3fa-463d-b5ac-11fb3a3bdd22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>